<commit_message>
updated NPC1 ExAC data
</commit_message>
<xml_diff>
--- a/mendelian_conservation/Protein_Data/NPC1.xlsx
+++ b/mendelian_conservation/Protein_Data/NPC1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="82">
   <si>
     <t>Gene </t>
   </si>
@@ -236,6 +236,39 @@
   </si>
   <si>
     <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=11182931</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=11754101</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=11349231</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=11333381</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=16126423</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=12955717</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=11545687</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=10521290</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=10521297</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=11479732</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=12401890</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=16098014</t>
   </si>
 </sst>
 </file>
@@ -250,6 +283,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -433,9 +467,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.780612244898"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2079,9 +2110,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.780612244898"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2458,9 +2486,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.780612244898"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2830,16 +2855,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.780612244898"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2890,6 +2912,12 @@
       <c r="B4" s="0" t="n">
         <v>7.46662</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -2898,6 +2926,12 @@
       <c r="B5" s="0" t="n">
         <v>6.97135</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -2906,6 +2940,18 @@
       <c r="B6" s="0" t="n">
         <v>6.54404</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
@@ -2922,6 +2968,12 @@
       <c r="B8" s="0" t="n">
         <v>6.12529</v>
       </c>
+      <c r="C8" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -2930,6 +2982,12 @@
       <c r="B9" s="0" t="n">
         <v>5.9662</v>
       </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
@@ -2938,6 +2996,18 @@
       <c r="B10" s="0" t="n">
         <v>5.93311</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -2946,6 +3016,39 @@
       <c r="B11" s="0" t="n">
         <v>5.46544</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -3025,6 +3128,12 @@
       </c>
       <c r="B21" s="0" t="n">
         <v>4.4106</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
got rid of unused code
</commit_message>
<xml_diff>
--- a/mendelian_conservation/Protein_Data/NPC1.xlsx
+++ b/mendelian_conservation/Protein_Data/NPC1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="983" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="87">
   <si>
     <t>Gene </t>
   </si>
@@ -269,6 +269,21 @@
   </si>
   <si>
     <t>http://www.ncbi.nlm.nih.gov/sites/entrez?db=pubmed&amp;cmd=search&amp;term=16098014</t>
+  </si>
+  <si>
+    <t>1 STDEV</t>
+  </si>
+  <si>
+    <t>2 STDEV</t>
+  </si>
+  <si>
+    <t>3 STDEV</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Stdev</t>
   </si>
 </sst>
 </file>
@@ -283,6 +298,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -300,7 +316,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,17 +326,41 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
-        <bgColor rgb="FF808080"/>
+        <bgColor rgb="FFB2B2B2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00CC33"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FF00CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009999"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCCC"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FFFF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -333,6 +373,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -361,7 +408,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,6 +426,30 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -406,13 +477,13 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF009999"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF99FFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -425,7 +496,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FF00CCCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
@@ -467,7 +538,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,7 +2184,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,7 +2563,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,15 +2934,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2888,11 +2959,11 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="5" t="n">
         <v>9.67517</v>
       </c>
       <c r="C2" s="2" t="n">
@@ -2902,11 +2973,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="5" t="n">
         <v>8.84458</v>
       </c>
       <c r="C3" s="2" t="n">
@@ -2916,11 +2987,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="6" t="n">
         <v>7.46662</v>
       </c>
       <c r="C4" s="2" t="n">
@@ -2930,11 +3001,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="6" t="n">
         <v>6.97135</v>
       </c>
       <c r="C5" s="2" t="n">
@@ -2944,11 +3015,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="6" t="n">
         <v>6.54404</v>
       </c>
       <c r="C6" s="2" t="n">
@@ -2964,19 +3035,19 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="6" t="n">
         <v>6.34791</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="7" t="n">
         <v>6.12529</v>
       </c>
       <c r="C8" s="2" t="n">
@@ -2986,11 +3057,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="7" t="n">
         <v>5.9662</v>
       </c>
       <c r="C9" s="2" t="n">
@@ -3000,11 +3071,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="7" t="n">
         <v>5.93311</v>
       </c>
       <c r="C10" s="2" t="n">
@@ -3020,11 +3091,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="7" t="n">
         <v>5.46544</v>
       </c>
       <c r="C11" s="2" t="n">
@@ -3061,83 +3132,83 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="7" t="n">
         <v>5.43495</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="7" t="n">
         <v>5.23831</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="7" t="n">
         <v>5.21643</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="7" t="n">
         <v>5.13544</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="7" t="n">
         <v>5.09602</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="7" t="n">
         <v>5.03873</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="7" t="n">
         <v>4.92797</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="7" t="n">
         <v>4.70598</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="7" t="n">
         <v>4.42816</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="7" t="n">
         <v>4.4106</v>
       </c>
       <c r="C21" s="2" t="n">
@@ -3147,196 +3218,247 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="7" t="n">
         <v>4.33581</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="7" t="n">
         <v>4.24988</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="7" t="n">
         <v>4.19267</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="7" t="n">
         <v>4.10533</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="7" t="n">
         <v>4.04492</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+    <row r="27" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="9" t="n">
         <v>4.03674</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="7" t="n">
         <v>3.85777</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="7" t="n">
         <v>3.60347</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="7" t="n">
         <v>3.59653</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="7" t="n">
         <v>3.21317</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="7" t="n">
         <v>2.5847</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="2" t="n">
+      <c r="B33" s="7" t="n">
         <v>2.35452</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="2" t="n">
+      <c r="B34" s="7" t="n">
         <v>2.25278</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="2" t="n">
+      <c r="B35" s="6" t="n">
         <v>1.06217</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="6" t="n">
         <v>1.03079</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="2" t="n">
+      <c r="B37" s="6" t="n">
         <v>0.85362</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="2" t="n">
+      <c r="B38" s="6" t="n">
         <v>0.8334</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="2" t="n">
+      <c r="B39" s="6" t="n">
         <v>0.80596</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="2" t="n">
+      <c r="B40" s="6" t="n">
         <v>0.72453</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="2" t="n">
+      <c r="B41" s="6" t="n">
         <v>0.6846</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="6" t="n">
         <v>0.67039</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="6" t="n">
         <v>0.59318</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="6" t="n">
         <v>0.1605</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D44" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="6" t="n">
         <v>-0.22357</v>
+      </c>
+      <c r="D45" s="10" t="n">
+        <f aca="false">B46+B47</f>
+        <v>6.31635717550195</v>
+      </c>
+      <c r="E45" s="10" t="n">
+        <f aca="false">B46+2*B47</f>
+        <v>8.7100743510039</v>
+      </c>
+      <c r="F45" s="10" t="n">
+        <f aca="false">B46+3*B47</f>
+        <v>11.1037915265058</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="10" t="n">
+        <f aca="false">AVERAGE(B2:B45)</f>
+        <v>3.92264</v>
+      </c>
+      <c r="D46" s="10" t="n">
+        <f aca="false">B46-B47</f>
+        <v>1.52892282449805</v>
+      </c>
+      <c r="E46" s="10" t="n">
+        <f aca="false">B46-2*B47</f>
+        <v>-0.864794351003896</v>
+      </c>
+      <c r="F46" s="10" t="n">
+        <f aca="false">B46-3*B47</f>
+        <v>-3.25851152650584</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="10" t="n">
+        <f aca="false">STDEV(B2:B45)</f>
+        <v>2.39371717550195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>